<commit_message>
Add new documents and fixed details
</commit_message>
<xml_diff>
--- a/utd/utils/output.xlsx
+++ b/utd/utils/output.xlsx
@@ -1315,7 +1315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fafba978-393b-4667-8984-c7b15454a66b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e88e9cb4-cfe7-4771-b2b1-1601eb72b8e6}">
   <dimension ref="A1:ZZ49"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -36289,7 +36289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872639d1-c576-4652-adf9-a07a8faa3d53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3a41d774-9ec9-4ff2-afda-b6c5ffa52cf2}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>